<commit_message>
Updated files from WRI China bringing the Hong Kong EPS up to v2.0.0
</commit_message>
<xml_diff>
--- a/InputData/add-outputs/SCoC/Social Cost of Carbon.xlsx
+++ b/InputData/add-outputs/SCoC/Social Cost of Carbon.xlsx
@@ -1,33 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_8810C517466EE2A53A5B737DA5F6823747F138A7" xr6:coauthVersionLast="42" xr6:coauthVersionMax="42" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipI\InputData\add-outputs\SCoC\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="21075" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="21075" windowHeight="11820"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="SourceData" sheetId="2" r:id="rId2"/>
     <sheet name="SCoC" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191028" iterate="1" iterateDelta="1.0000000000000001E-5"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
-  <si>
-    <t>SCoC Social Cost of Carbon</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t>Source:</t>
   </si>
@@ -38,16 +32,31 @@
     <t>Technical Update of the Social Cost of Carbon for Regulatory Impact Analysis</t>
   </si>
   <si>
-    <t>https://www.whitehouse.gov/sites/default/files/omb/inforeg/scc-tsd-final-july-2015.pdf</t>
+    <t>Discount Rate</t>
   </si>
   <si>
-    <t>Page 17, Table A1</t>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Percentile</t>
+  </si>
+  <si>
+    <t>Avg</t>
+  </si>
+  <si>
+    <t>95th%</t>
+  </si>
+  <si>
+    <t>Source Data in 2007 dollars/metric ton CO2</t>
+  </si>
+  <si>
+    <t>Data in 2012 dollars/gram CO2</t>
+  </si>
+  <si>
+    <t>SCoC Social Cost of Carbon</t>
   </si>
   <si>
     <t>Notes:</t>
-  </si>
-  <si>
-    <t>When considering the Social Cost of Carbon, the U.S. government typically uses the figures based on</t>
   </si>
   <si>
     <t>a 3% discount rate, so this is the rate we use in this model.</t>
@@ -59,45 +68,36 @@
     <t>based on the Office of Management and Budget guidelines for analysis of prospective investments and policies.</t>
   </si>
   <si>
+    <t>See "cpi.xlsx" in the InputData folder for source information.</t>
+  </si>
+  <si>
     <t>We adjust 2007 dollars to 2012 dollars using the following conversion factor:</t>
   </si>
   <si>
-    <t>See "cpi.xlsx" in the InputData folder for source information.</t>
+    <t>Page 17, Table A1</t>
   </si>
   <si>
-    <t>Source Data in 2007 dollars/metric ton CO2</t>
+    <t>https://www.whitehouse.gov/sites/default/files/omb/inforeg/scc-tsd-final-july-2015.pdf</t>
   </si>
   <si>
-    <t>Data in 2012 dollars/gram CO2</t>
+    <t>Social Cost of Carbon ($/g CO2e)</t>
   </si>
   <si>
-    <t>Discount Rate</t>
+    <t>When considering the Social Cost of Carbon, meant to capture the long-term economic damage caused by one</t>
   </si>
   <si>
-    <t>Percentile</t>
-  </si>
-  <si>
-    <t>Avg</t>
-  </si>
-  <si>
-    <t>95th%</t>
-  </si>
-  <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t>Social Cost of Carbon ($)</t>
+    <t>ton of carbon dioxide emitted, the U.S. government typically uses the figures based on</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -259,14 +259,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="8">
-    <cellStyle name="Body: normal cell" xfId="5" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Footnotes: top row" xfId="7" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Header: bottom row" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Body: normal cell" xfId="5"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="3"/>
+    <cellStyle name="Footnotes: top row" xfId="7"/>
+    <cellStyle name="Header: bottom row" xfId="4"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Parent row" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="Table title" xfId="2" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Parent row" xfId="6"/>
+    <cellStyle name="Table title" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -357,23 +357,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -409,23 +392,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -601,99 +567,94 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="97.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="1" t="s">
+      <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="13" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="13"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>2015</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="13"/>
-      <c r="B5" s="13" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="13"/>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="13"/>
-      <c r="B7" s="13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="13"/>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="13"/>
-    </row>
-    <row r="11" spans="1:2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="13"/>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="13"/>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="13"/>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="13"/>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="13">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="13">
         <v>1.109</v>
       </c>
-      <c r="B16" s="13"/>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="13" t="s">
-        <v>12</v>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="13" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -703,37 +664,36 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.42578125" customWidth="1"/>
     <col min="7" max="7" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
-      <c r="F1" s="13"/>
       <c r="G1" s="10" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="H1" s="11"/>
       <c r="I1" s="11"/>
       <c r="J1" s="11"/>
       <c r="K1" s="11"/>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B2" s="4">
         <v>0.05</v>
@@ -747,9 +707,8 @@
       <c r="E2" s="4">
         <v>0.03</v>
       </c>
-      <c r="F2" s="13"/>
       <c r="G2" s="5" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="H2" s="4">
         <v>0.05</v>
@@ -764,40 +723,39 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="13"/>
+        <v>7</v>
+      </c>
       <c r="G3" s="5" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="13">
         <v>2010</v>
       </c>
@@ -813,29 +771,28 @@
       <c r="E4" s="7">
         <v>86</v>
       </c>
-      <c r="F4" s="13"/>
       <c r="G4" s="1">
         <f>A4</f>
         <v>2010</v>
       </c>
       <c r="H4" s="12">
-        <f>B4*(About!$A$16)/10^6</f>
+        <f>B4*(About!$A$17)/10^6</f>
         <v>1.1090000000000001E-5</v>
       </c>
       <c r="I4" s="12">
-        <f>C4*(About!$A$16)/10^6</f>
+        <f>C4*(About!$A$17)/10^6</f>
         <v>3.4378999999999997E-5</v>
       </c>
       <c r="J4" s="12">
-        <f>D4*(About!$A$16)/10^6</f>
+        <f>D4*(About!$A$17)/10^6</f>
         <v>5.5450000000000006E-5</v>
       </c>
       <c r="K4" s="12">
-        <f>E4*(About!$A$16)/10^6</f>
+        <f>E4*(About!$A$17)/10^6</f>
         <v>9.5373999999999999E-5</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="13">
         <v>2011</v>
       </c>
@@ -851,29 +808,28 @@
       <c r="E5" s="7">
         <v>90</v>
       </c>
-      <c r="F5" s="13"/>
       <c r="G5" s="1">
         <f t="shared" ref="G5:G44" si="0">A5</f>
         <v>2011</v>
       </c>
       <c r="H5" s="12">
-        <f>B5*(About!$A$16)/10^6</f>
+        <f>B5*(About!$A$17)/10^6</f>
         <v>1.2199E-5</v>
       </c>
       <c r="I5" s="12">
-        <f>C5*(About!$A$16)/10^6</f>
+        <f>C5*(About!$A$17)/10^6</f>
         <v>3.5487999999999996E-5</v>
       </c>
       <c r="J5" s="12">
-        <f>D5*(About!$A$16)/10^6</f>
+        <f>D5*(About!$A$17)/10^6</f>
         <v>5.6558999999999998E-5</v>
       </c>
       <c r="K5" s="12">
-        <f>E5*(About!$A$16)/10^6</f>
+        <f>E5*(About!$A$17)/10^6</f>
         <v>9.9810000000000008E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
         <v>2012</v>
       </c>
@@ -889,29 +845,28 @@
       <c r="E6" s="7">
         <v>93</v>
       </c>
-      <c r="F6" s="13"/>
       <c r="G6" s="1">
         <f t="shared" si="0"/>
         <v>2012</v>
       </c>
       <c r="H6" s="12">
-        <f>B6*(About!$A$16)/10^6</f>
+        <f>B6*(About!$A$17)/10^6</f>
         <v>1.2199E-5</v>
       </c>
       <c r="I6" s="12">
-        <f>C6*(About!$A$16)/10^6</f>
+        <f>C6*(About!$A$17)/10^6</f>
         <v>3.6597000000000002E-5</v>
       </c>
       <c r="J6" s="12">
-        <f>D6*(About!$A$16)/10^6</f>
+        <f>D6*(About!$A$17)/10^6</f>
         <v>5.8777000000000003E-5</v>
       </c>
       <c r="K6" s="12">
-        <f>E6*(About!$A$16)/10^6</f>
+        <f>E6*(About!$A$17)/10^6</f>
         <v>1.03137E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="13">
         <v>2013</v>
       </c>
@@ -927,29 +882,28 @@
       <c r="E7" s="7">
         <v>97</v>
       </c>
-      <c r="F7" s="13"/>
       <c r="G7" s="1">
         <f t="shared" si="0"/>
         <v>2013</v>
       </c>
       <c r="H7" s="12">
-        <f>B7*(About!$A$16)/10^6</f>
+        <f>B7*(About!$A$17)/10^6</f>
         <v>1.2199E-5</v>
       </c>
       <c r="I7" s="12">
-        <f>C7*(About!$A$16)/10^6</f>
+        <f>C7*(About!$A$17)/10^6</f>
         <v>3.7706000000000001E-5</v>
       </c>
       <c r="J7" s="12">
-        <f>D7*(About!$A$16)/10^6</f>
+        <f>D7*(About!$A$17)/10^6</f>
         <v>5.9885999999999995E-5</v>
       </c>
       <c r="K7" s="12">
-        <f>E7*(About!$A$16)/10^6</f>
+        <f>E7*(About!$A$17)/10^6</f>
         <v>1.0757299999999999E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="13">
         <v>2014</v>
       </c>
@@ -965,29 +919,28 @@
       <c r="E8" s="7">
         <v>101</v>
       </c>
-      <c r="F8" s="13"/>
       <c r="G8" s="1">
         <f t="shared" si="0"/>
         <v>2014</v>
       </c>
       <c r="H8" s="12">
-        <f>B8*(About!$A$16)/10^6</f>
+        <f>B8*(About!$A$17)/10^6</f>
         <v>1.2199E-5</v>
       </c>
       <c r="I8" s="12">
-        <f>C8*(About!$A$16)/10^6</f>
+        <f>C8*(About!$A$17)/10^6</f>
         <v>3.8815E-5</v>
       </c>
       <c r="J8" s="12">
-        <f>D8*(About!$A$16)/10^6</f>
+        <f>D8*(About!$A$17)/10^6</f>
         <v>6.0994999999999995E-5</v>
       </c>
       <c r="K8" s="12">
-        <f>E8*(About!$A$16)/10^6</f>
+        <f>E8*(About!$A$17)/10^6</f>
         <v>1.12009E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="13">
         <v>2015</v>
       </c>
@@ -1003,29 +956,28 @@
       <c r="E9" s="7">
         <v>105</v>
       </c>
-      <c r="F9" s="13"/>
       <c r="G9" s="1">
         <f t="shared" si="0"/>
         <v>2015</v>
       </c>
       <c r="H9" s="12">
-        <f>B9*(About!$A$16)/10^6</f>
+        <f>B9*(About!$A$17)/10^6</f>
         <v>1.2199E-5</v>
       </c>
       <c r="I9" s="12">
-        <f>C9*(About!$A$16)/10^6</f>
+        <f>C9*(About!$A$17)/10^6</f>
         <v>3.9923999999999999E-5</v>
       </c>
       <c r="J9" s="12">
-        <f>D9*(About!$A$16)/10^6</f>
+        <f>D9*(About!$A$17)/10^6</f>
         <v>6.2104E-5</v>
       </c>
       <c r="K9" s="12">
-        <f>E9*(About!$A$16)/10^6</f>
+        <f>E9*(About!$A$17)/10^6</f>
         <v>1.1644499999999999E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="13">
         <v>2016</v>
       </c>
@@ -1041,29 +993,28 @@
       <c r="E10" s="7">
         <v>108</v>
       </c>
-      <c r="F10" s="13"/>
       <c r="G10" s="1">
         <f t="shared" si="0"/>
         <v>2016</v>
       </c>
       <c r="H10" s="12">
-        <f>B10*(About!$A$16)/10^6</f>
+        <f>B10*(About!$A$17)/10^6</f>
         <v>1.2199E-5</v>
       </c>
       <c r="I10" s="12">
-        <f>C10*(About!$A$16)/10^6</f>
+        <f>C10*(About!$A$17)/10^6</f>
         <v>4.2141999999999997E-5</v>
       </c>
       <c r="J10" s="12">
-        <f>D10*(About!$A$16)/10^6</f>
+        <f>D10*(About!$A$17)/10^6</f>
         <v>6.3213000000000006E-5</v>
       </c>
       <c r="K10" s="12">
-        <f>E10*(About!$A$16)/10^6</f>
+        <f>E10*(About!$A$17)/10^6</f>
         <v>1.1977199999999999E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="13">
         <v>2017</v>
       </c>
@@ -1079,29 +1030,28 @@
       <c r="E11" s="7">
         <v>112</v>
       </c>
-      <c r="F11" s="13"/>
       <c r="G11" s="1">
         <f t="shared" si="0"/>
         <v>2017</v>
       </c>
       <c r="H11" s="12">
-        <f>B11*(About!$A$16)/10^6</f>
+        <f>B11*(About!$A$17)/10^6</f>
         <v>1.2199E-5</v>
       </c>
       <c r="I11" s="12">
-        <f>C11*(About!$A$16)/10^6</f>
+        <f>C11*(About!$A$17)/10^6</f>
         <v>4.3250999999999996E-5</v>
       </c>
       <c r="J11" s="12">
-        <f>D11*(About!$A$16)/10^6</f>
+        <f>D11*(About!$A$17)/10^6</f>
         <v>6.5430999999999991E-5</v>
       </c>
       <c r="K11" s="12">
-        <f>E11*(About!$A$16)/10^6</f>
+        <f>E11*(About!$A$17)/10^6</f>
         <v>1.24208E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="13">
         <v>2018</v>
       </c>
@@ -1117,29 +1067,28 @@
       <c r="E12" s="7">
         <v>116</v>
       </c>
-      <c r="F12" s="13"/>
       <c r="G12" s="1">
         <f t="shared" si="0"/>
         <v>2018</v>
       </c>
       <c r="H12" s="12">
-        <f>B12*(About!$A$16)/10^6</f>
+        <f>B12*(About!$A$17)/10^6</f>
         <v>1.3308E-5</v>
       </c>
       <c r="I12" s="12">
-        <f>C12*(About!$A$16)/10^6</f>
+        <f>C12*(About!$A$17)/10^6</f>
         <v>4.4360000000000002E-5</v>
       </c>
       <c r="J12" s="12">
-        <f>D12*(About!$A$16)/10^6</f>
+        <f>D12*(About!$A$17)/10^6</f>
         <v>6.6539999999999997E-5</v>
       </c>
       <c r="K12" s="12">
-        <f>E12*(About!$A$16)/10^6</f>
+        <f>E12*(About!$A$17)/10^6</f>
         <v>1.28644E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="13">
         <v>2019</v>
       </c>
@@ -1155,29 +1104,28 @@
       <c r="E13" s="7">
         <v>120</v>
       </c>
-      <c r="F13" s="13"/>
       <c r="G13" s="1">
         <f t="shared" si="0"/>
         <v>2019</v>
       </c>
       <c r="H13" s="12">
-        <f>B13*(About!$A$16)/10^6</f>
+        <f>B13*(About!$A$17)/10^6</f>
         <v>1.3308E-5</v>
       </c>
       <c r="I13" s="12">
-        <f>C13*(About!$A$16)/10^6</f>
+        <f>C13*(About!$A$17)/10^6</f>
         <v>4.5469000000000001E-5</v>
       </c>
       <c r="J13" s="12">
-        <f>D13*(About!$A$16)/10^6</f>
+        <f>D13*(About!$A$17)/10^6</f>
         <v>6.7649000000000002E-5</v>
       </c>
       <c r="K13" s="12">
-        <f>E13*(About!$A$16)/10^6</f>
+        <f>E13*(About!$A$17)/10^6</f>
         <v>1.3307999999999999E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="13">
         <v>2020</v>
       </c>
@@ -1193,29 +1141,28 @@
       <c r="E14" s="7">
         <v>123</v>
       </c>
-      <c r="F14" s="13"/>
       <c r="G14" s="1">
         <f t="shared" si="0"/>
         <v>2020</v>
       </c>
       <c r="H14" s="12">
-        <f>B14*(About!$A$16)/10^6</f>
+        <f>B14*(About!$A$17)/10^6</f>
         <v>1.3308E-5</v>
       </c>
       <c r="I14" s="12">
-        <f>C14*(About!$A$16)/10^6</f>
+        <f>C14*(About!$A$17)/10^6</f>
         <v>4.6578E-5</v>
       </c>
       <c r="J14" s="12">
-        <f>D14*(About!$A$16)/10^6</f>
+        <f>D14*(About!$A$17)/10^6</f>
         <v>6.8757999999999995E-5</v>
       </c>
       <c r="K14" s="12">
-        <f>E14*(About!$A$16)/10^6</f>
+        <f>E14*(About!$A$17)/10^6</f>
         <v>1.3640700000000001E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="13">
         <v>2021</v>
       </c>
@@ -1231,29 +1178,28 @@
       <c r="E15" s="7">
         <v>126</v>
       </c>
-      <c r="F15" s="13"/>
       <c r="G15" s="1">
         <f t="shared" si="0"/>
         <v>2021</v>
       </c>
       <c r="H15" s="12">
-        <f>B15*(About!$A$16)/10^6</f>
+        <f>B15*(About!$A$17)/10^6</f>
         <v>1.3308E-5</v>
       </c>
       <c r="I15" s="12">
-        <f>C15*(About!$A$16)/10^6</f>
+        <f>C15*(About!$A$17)/10^6</f>
         <v>4.6578E-5</v>
       </c>
       <c r="J15" s="12">
-        <f>D15*(About!$A$16)/10^6</f>
+        <f>D15*(About!$A$17)/10^6</f>
         <v>6.9867E-5</v>
       </c>
       <c r="K15" s="12">
-        <f>E15*(About!$A$16)/10^6</f>
+        <f>E15*(About!$A$17)/10^6</f>
         <v>1.39734E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="13">
         <v>2022</v>
       </c>
@@ -1269,29 +1215,28 @@
       <c r="E16" s="7">
         <v>129</v>
       </c>
-      <c r="F16" s="13"/>
       <c r="G16" s="1">
         <f t="shared" si="0"/>
         <v>2022</v>
       </c>
       <c r="H16" s="12">
-        <f>B16*(About!$A$16)/10^6</f>
+        <f>B16*(About!$A$17)/10^6</f>
         <v>1.4416999999999999E-5</v>
       </c>
       <c r="I16" s="12">
-        <f>C16*(About!$A$16)/10^6</f>
+        <f>C16*(About!$A$17)/10^6</f>
         <v>4.7686999999999999E-5</v>
       </c>
       <c r="J16" s="12">
-        <f>D16*(About!$A$16)/10^6</f>
+        <f>D16*(About!$A$17)/10^6</f>
         <v>7.0975999999999993E-5</v>
       </c>
       <c r="K16" s="12">
-        <f>E16*(About!$A$16)/10^6</f>
+        <f>E16*(About!$A$17)/10^6</f>
         <v>1.4306100000000002E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="13">
         <v>2023</v>
       </c>
@@ -1307,29 +1252,28 @@
       <c r="E17" s="7">
         <v>132</v>
       </c>
-      <c r="F17" s="13"/>
       <c r="G17" s="1">
         <f t="shared" si="0"/>
         <v>2023</v>
       </c>
       <c r="H17" s="12">
-        <f>B17*(About!$A$16)/10^6</f>
+        <f>B17*(About!$A$17)/10^6</f>
         <v>1.4416999999999999E-5</v>
       </c>
       <c r="I17" s="12">
-        <f>C17*(About!$A$16)/10^6</f>
+        <f>C17*(About!$A$17)/10^6</f>
         <v>4.8795999999999998E-5</v>
       </c>
       <c r="J17" s="12">
-        <f>D17*(About!$A$16)/10^6</f>
+        <f>D17*(About!$A$17)/10^6</f>
         <v>7.2084999999999998E-5</v>
       </c>
       <c r="K17" s="12">
-        <f>E17*(About!$A$16)/10^6</f>
+        <f>E17*(About!$A$17)/10^6</f>
         <v>1.4638800000000001E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="13">
         <v>2024</v>
       </c>
@@ -1345,29 +1289,28 @@
       <c r="E18" s="7">
         <v>135</v>
       </c>
-      <c r="F18" s="13"/>
       <c r="G18" s="1">
         <f t="shared" si="0"/>
         <v>2024</v>
       </c>
       <c r="H18" s="12">
-        <f>B18*(About!$A$16)/10^6</f>
+        <f>B18*(About!$A$17)/10^6</f>
         <v>1.4416999999999999E-5</v>
       </c>
       <c r="I18" s="12">
-        <f>C18*(About!$A$16)/10^6</f>
+        <f>C18*(About!$A$17)/10^6</f>
         <v>4.9905000000000004E-5</v>
       </c>
       <c r="J18" s="12">
-        <f>D18*(About!$A$16)/10^6</f>
+        <f>D18*(About!$A$17)/10^6</f>
         <v>7.3194000000000004E-5</v>
       </c>
       <c r="K18" s="12">
-        <f>E18*(About!$A$16)/10^6</f>
+        <f>E18*(About!$A$17)/10^6</f>
         <v>1.49715E-4</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="13">
         <v>2025</v>
       </c>
@@ -1383,29 +1326,28 @@
       <c r="E19" s="7">
         <v>138</v>
       </c>
-      <c r="F19" s="13"/>
       <c r="G19" s="1">
         <f t="shared" si="0"/>
         <v>2025</v>
       </c>
       <c r="H19" s="12">
-        <f>B19*(About!$A$16)/10^6</f>
+        <f>B19*(About!$A$17)/10^6</f>
         <v>1.5526E-5</v>
       </c>
       <c r="I19" s="12">
-        <f>C19*(About!$A$16)/10^6</f>
+        <f>C19*(About!$A$17)/10^6</f>
         <v>5.1013999999999996E-5</v>
       </c>
       <c r="J19" s="12">
-        <f>D19*(About!$A$16)/10^6</f>
+        <f>D19*(About!$A$17)/10^6</f>
         <v>7.5412000000000002E-5</v>
       </c>
       <c r="K19" s="12">
-        <f>E19*(About!$A$16)/10^6</f>
+        <f>E19*(About!$A$17)/10^6</f>
         <v>1.5304199999999999E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="13">
         <v>2026</v>
       </c>
@@ -1421,29 +1363,28 @@
       <c r="E20" s="7">
         <v>141</v>
       </c>
-      <c r="F20" s="13"/>
       <c r="G20" s="1">
         <f t="shared" si="0"/>
         <v>2026</v>
       </c>
       <c r="H20" s="12">
-        <f>B20*(About!$A$16)/10^6</f>
+        <f>B20*(About!$A$17)/10^6</f>
         <v>1.5526E-5</v>
       </c>
       <c r="I20" s="12">
-        <f>C20*(About!$A$16)/10^6</f>
+        <f>C20*(About!$A$17)/10^6</f>
         <v>5.2122999999999995E-5</v>
       </c>
       <c r="J20" s="12">
-        <f>D20*(About!$A$16)/10^6</f>
+        <f>D20*(About!$A$17)/10^6</f>
         <v>7.6520999999999995E-5</v>
       </c>
       <c r="K20" s="12">
-        <f>E20*(About!$A$16)/10^6</f>
+        <f>E20*(About!$A$17)/10^6</f>
         <v>1.5636900000000001E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="13">
         <v>2027</v>
       </c>
@@ -1459,29 +1400,28 @@
       <c r="E21" s="7">
         <v>143</v>
       </c>
-      <c r="F21" s="13"/>
       <c r="G21" s="1">
         <f t="shared" si="0"/>
         <v>2027</v>
       </c>
       <c r="H21" s="12">
-        <f>B21*(About!$A$16)/10^6</f>
+        <f>B21*(About!$A$17)/10^6</f>
         <v>1.6634999999999999E-5</v>
       </c>
       <c r="I21" s="12">
-        <f>C21*(About!$A$16)/10^6</f>
+        <f>C21*(About!$A$17)/10^6</f>
         <v>5.3232000000000001E-5</v>
       </c>
       <c r="J21" s="12">
-        <f>D21*(About!$A$16)/10^6</f>
+        <f>D21*(About!$A$17)/10^6</f>
         <v>7.763E-5</v>
       </c>
       <c r="K21" s="12">
-        <f>E21*(About!$A$16)/10^6</f>
+        <f>E21*(About!$A$17)/10^6</f>
         <v>1.5858699999999999E-4</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="13">
         <v>2028</v>
       </c>
@@ -1497,29 +1437,28 @@
       <c r="E22" s="7">
         <v>146</v>
       </c>
-      <c r="F22" s="13"/>
       <c r="G22" s="1">
         <f t="shared" si="0"/>
         <v>2028</v>
       </c>
       <c r="H22" s="12">
-        <f>B22*(About!$A$16)/10^6</f>
+        <f>B22*(About!$A$17)/10^6</f>
         <v>1.6634999999999999E-5</v>
       </c>
       <c r="I22" s="12">
-        <f>C22*(About!$A$16)/10^6</f>
+        <f>C22*(About!$A$17)/10^6</f>
         <v>5.4341E-5</v>
       </c>
       <c r="J22" s="12">
-        <f>D22*(About!$A$16)/10^6</f>
+        <f>D22*(About!$A$17)/10^6</f>
         <v>7.8739000000000006E-5</v>
       </c>
       <c r="K22" s="12">
-        <f>E22*(About!$A$16)/10^6</f>
+        <f>E22*(About!$A$17)/10^6</f>
         <v>1.6191399999999998E-4</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="13">
         <v>2029</v>
       </c>
@@ -1535,29 +1474,28 @@
       <c r="E23" s="7">
         <v>149</v>
       </c>
-      <c r="F23" s="13"/>
       <c r="G23" s="1">
         <f t="shared" si="0"/>
         <v>2029</v>
       </c>
       <c r="H23" s="12">
-        <f>B23*(About!$A$16)/10^6</f>
+        <f>B23*(About!$A$17)/10^6</f>
         <v>1.6634999999999999E-5</v>
       </c>
       <c r="I23" s="12">
-        <f>C23*(About!$A$16)/10^6</f>
+        <f>C23*(About!$A$17)/10^6</f>
         <v>5.4341E-5</v>
       </c>
       <c r="J23" s="12">
-        <f>D23*(About!$A$16)/10^6</f>
+        <f>D23*(About!$A$17)/10^6</f>
         <v>7.9847999999999999E-5</v>
       </c>
       <c r="K23" s="12">
-        <f>E23*(About!$A$16)/10^6</f>
+        <f>E23*(About!$A$17)/10^6</f>
         <v>1.65241E-4</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="13">
         <v>2030</v>
       </c>
@@ -1573,29 +1511,28 @@
       <c r="E24" s="7">
         <v>152</v>
       </c>
-      <c r="F24" s="13"/>
       <c r="G24" s="1">
         <f t="shared" si="0"/>
         <v>2030</v>
       </c>
       <c r="H24" s="12">
-        <f>B24*(About!$A$16)/10^6</f>
+        <f>B24*(About!$A$17)/10^6</f>
         <v>1.7743999999999998E-5</v>
       </c>
       <c r="I24" s="12">
-        <f>C24*(About!$A$16)/10^6</f>
+        <f>C24*(About!$A$17)/10^6</f>
         <v>5.5450000000000006E-5</v>
       </c>
       <c r="J24" s="12">
-        <f>D24*(About!$A$16)/10^6</f>
+        <f>D24*(About!$A$17)/10^6</f>
         <v>8.0956999999999991E-5</v>
       </c>
       <c r="K24" s="12">
-        <f>E24*(About!$A$16)/10^6</f>
+        <f>E24*(About!$A$17)/10^6</f>
         <v>1.6856799999999999E-4</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="13">
         <v>2031</v>
       </c>
@@ -1611,29 +1548,28 @@
       <c r="E25" s="7">
         <v>155</v>
       </c>
-      <c r="F25" s="13"/>
       <c r="G25" s="1">
         <f t="shared" si="0"/>
         <v>2031</v>
       </c>
       <c r="H25" s="12">
-        <f>B25*(About!$A$16)/10^6</f>
+        <f>B25*(About!$A$17)/10^6</f>
         <v>1.7743999999999998E-5</v>
       </c>
       <c r="I25" s="12">
-        <f>C25*(About!$A$16)/10^6</f>
+        <f>C25*(About!$A$17)/10^6</f>
         <v>5.6558999999999998E-5</v>
       </c>
       <c r="J25" s="12">
-        <f>D25*(About!$A$16)/10^6</f>
+        <f>D25*(About!$A$17)/10^6</f>
         <v>8.2065999999999997E-5</v>
       </c>
       <c r="K25" s="12">
-        <f>E25*(About!$A$16)/10^6</f>
+        <f>E25*(About!$A$17)/10^6</f>
         <v>1.7189500000000001E-4</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="13">
         <v>2032</v>
       </c>
@@ -1649,29 +1585,28 @@
       <c r="E26" s="7">
         <v>158</v>
       </c>
-      <c r="F26" s="13"/>
       <c r="G26" s="1">
         <f t="shared" si="0"/>
         <v>2032</v>
       </c>
       <c r="H26" s="12">
-        <f>B26*(About!$A$16)/10^6</f>
+        <f>B26*(About!$A$17)/10^6</f>
         <v>1.8853000000000001E-5</v>
       </c>
       <c r="I26" s="12">
-        <f>C26*(About!$A$16)/10^6</f>
+        <f>C26*(About!$A$17)/10^6</f>
         <v>5.7667999999999997E-5</v>
       </c>
       <c r="J26" s="12">
-        <f>D26*(About!$A$16)/10^6</f>
+        <f>D26*(About!$A$17)/10^6</f>
         <v>8.3175000000000002E-5</v>
       </c>
       <c r="K26" s="12">
-        <f>E26*(About!$A$16)/10^6</f>
+        <f>E26*(About!$A$17)/10^6</f>
         <v>1.75222E-4</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="13">
         <v>2033</v>
       </c>
@@ -1687,29 +1622,28 @@
       <c r="E27" s="7">
         <v>161</v>
       </c>
-      <c r="F27" s="13"/>
       <c r="G27" s="1">
         <f t="shared" si="0"/>
         <v>2033</v>
       </c>
       <c r="H27" s="12">
-        <f>B27*(About!$A$16)/10^6</f>
+        <f>B27*(About!$A$17)/10^6</f>
         <v>1.8853000000000001E-5</v>
       </c>
       <c r="I27" s="12">
-        <f>C27*(About!$A$16)/10^6</f>
+        <f>C27*(About!$A$17)/10^6</f>
         <v>5.8777000000000003E-5</v>
       </c>
       <c r="J27" s="12">
-        <f>D27*(About!$A$16)/10^6</f>
+        <f>D27*(About!$A$17)/10^6</f>
         <v>8.4283999999999995E-5</v>
       </c>
       <c r="K27" s="12">
-        <f>E27*(About!$A$16)/10^6</f>
+        <f>E27*(About!$A$17)/10^6</f>
         <v>1.7854900000000001E-4</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="13">
         <v>2034</v>
       </c>
@@ -1725,29 +1659,28 @@
       <c r="E28" s="7">
         <v>164</v>
       </c>
-      <c r="F28" s="13"/>
       <c r="G28" s="1">
         <f t="shared" si="0"/>
         <v>2034</v>
       </c>
       <c r="H28" s="12">
-        <f>B28*(About!$A$16)/10^6</f>
+        <f>B28*(About!$A$17)/10^6</f>
         <v>1.9962E-5</v>
       </c>
       <c r="I28" s="12">
-        <f>C28*(About!$A$16)/10^6</f>
+        <f>C28*(About!$A$17)/10^6</f>
         <v>5.9885999999999995E-5</v>
       </c>
       <c r="J28" s="12">
-        <f>D28*(About!$A$16)/10^6</f>
+        <f>D28*(About!$A$17)/10^6</f>
         <v>8.5393E-5</v>
       </c>
       <c r="K28" s="12">
-        <f>E28*(About!$A$16)/10^6</f>
+        <f>E28*(About!$A$17)/10^6</f>
         <v>1.81876E-4</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="13">
         <v>2035</v>
       </c>
@@ -1763,29 +1696,28 @@
       <c r="E29" s="7">
         <v>168</v>
       </c>
-      <c r="F29" s="13"/>
       <c r="G29" s="1">
         <f t="shared" si="0"/>
         <v>2035</v>
       </c>
       <c r="H29" s="12">
-        <f>B29*(About!$A$16)/10^6</f>
+        <f>B29*(About!$A$17)/10^6</f>
         <v>1.9962E-5</v>
       </c>
       <c r="I29" s="12">
-        <f>C29*(About!$A$16)/10^6</f>
+        <f>C29*(About!$A$17)/10^6</f>
         <v>6.0994999999999995E-5</v>
       </c>
       <c r="J29" s="12">
-        <f>D29*(About!$A$16)/10^6</f>
+        <f>D29*(About!$A$17)/10^6</f>
         <v>8.6501999999999993E-5</v>
       </c>
       <c r="K29" s="12">
-        <f>E29*(About!$A$16)/10^6</f>
+        <f>E29*(About!$A$17)/10^6</f>
         <v>1.86312E-4</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="13">
         <v>2036</v>
       </c>
@@ -1801,29 +1733,28 @@
       <c r="E30" s="7">
         <v>171</v>
       </c>
-      <c r="F30" s="13"/>
       <c r="G30" s="1">
         <f t="shared" si="0"/>
         <v>2036</v>
       </c>
       <c r="H30" s="12">
-        <f>B30*(About!$A$16)/10^6</f>
+        <f>B30*(About!$A$17)/10^6</f>
         <v>2.1070999999999999E-5</v>
       </c>
       <c r="I30" s="12">
-        <f>C30*(About!$A$16)/10^6</f>
+        <f>C30*(About!$A$17)/10^6</f>
         <v>6.2104E-5</v>
       </c>
       <c r="J30" s="12">
-        <f>D30*(About!$A$16)/10^6</f>
+        <f>D30*(About!$A$17)/10^6</f>
         <v>8.7610999999999999E-5</v>
       </c>
       <c r="K30" s="12">
-        <f>E30*(About!$A$16)/10^6</f>
+        <f>E30*(About!$A$17)/10^6</f>
         <v>1.8963900000000002E-4</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="13">
         <v>2037</v>
       </c>
@@ -1839,29 +1770,28 @@
       <c r="E31" s="7">
         <v>174</v>
       </c>
-      <c r="F31" s="13"/>
       <c r="G31" s="1">
         <f t="shared" si="0"/>
         <v>2037</v>
       </c>
       <c r="H31" s="12">
-        <f>B31*(About!$A$16)/10^6</f>
+        <f>B31*(About!$A$17)/10^6</f>
         <v>2.1070999999999999E-5</v>
       </c>
       <c r="I31" s="12">
-        <f>C31*(About!$A$16)/10^6</f>
+        <f>C31*(About!$A$17)/10^6</f>
         <v>6.3213000000000006E-5</v>
       </c>
       <c r="J31" s="12">
-        <f>D31*(About!$A$16)/10^6</f>
+        <f>D31*(About!$A$17)/10^6</f>
         <v>8.9828999999999997E-5</v>
       </c>
       <c r="K31" s="12">
-        <f>E31*(About!$A$16)/10^6</f>
+        <f>E31*(About!$A$17)/10^6</f>
         <v>1.9296600000000001E-4</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="13">
         <v>2038</v>
       </c>
@@ -1877,29 +1807,28 @@
       <c r="E32" s="7">
         <v>177</v>
       </c>
-      <c r="F32" s="13"/>
       <c r="G32" s="1">
         <f t="shared" si="0"/>
         <v>2038</v>
       </c>
       <c r="H32" s="12">
-        <f>B32*(About!$A$16)/10^6</f>
+        <f>B32*(About!$A$17)/10^6</f>
         <v>2.2180000000000001E-5</v>
       </c>
       <c r="I32" s="12">
-        <f>C32*(About!$A$16)/10^6</f>
+        <f>C32*(About!$A$17)/10^6</f>
         <v>6.4321999999999998E-5</v>
       </c>
       <c r="J32" s="12">
-        <f>D32*(About!$A$16)/10^6</f>
+        <f>D32*(About!$A$17)/10^6</f>
         <v>9.0938000000000002E-5</v>
       </c>
       <c r="K32" s="12">
-        <f>E32*(About!$A$16)/10^6</f>
+        <f>E32*(About!$A$17)/10^6</f>
         <v>1.96293E-4</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="13">
         <v>2039</v>
       </c>
@@ -1915,29 +1844,28 @@
       <c r="E33" s="7">
         <v>180</v>
       </c>
-      <c r="F33" s="13"/>
       <c r="G33" s="1">
         <f t="shared" si="0"/>
         <v>2039</v>
       </c>
       <c r="H33" s="12">
-        <f>B33*(About!$A$16)/10^6</f>
+        <f>B33*(About!$A$17)/10^6</f>
         <v>2.2180000000000001E-5</v>
       </c>
       <c r="I33" s="12">
-        <f>C33*(About!$A$16)/10^6</f>
+        <f>C33*(About!$A$17)/10^6</f>
         <v>6.5430999999999991E-5</v>
       </c>
       <c r="J33" s="12">
-        <f>D33*(About!$A$16)/10^6</f>
+        <f>D33*(About!$A$17)/10^6</f>
         <v>9.2046999999999995E-5</v>
       </c>
       <c r="K33" s="12">
-        <f>E33*(About!$A$16)/10^6</f>
+        <f>E33*(About!$A$17)/10^6</f>
         <v>1.9962000000000002E-4</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="13">
         <v>2040</v>
       </c>
@@ -1953,29 +1881,28 @@
       <c r="E34" s="7">
         <v>183</v>
       </c>
-      <c r="F34" s="13"/>
       <c r="G34" s="1">
         <f t="shared" si="0"/>
         <v>2040</v>
       </c>
       <c r="H34" s="12">
-        <f>B34*(About!$A$16)/10^6</f>
+        <f>B34*(About!$A$17)/10^6</f>
         <v>2.3289E-5</v>
       </c>
       <c r="I34" s="12">
-        <f>C34*(About!$A$16)/10^6</f>
+        <f>C34*(About!$A$17)/10^6</f>
         <v>6.6539999999999997E-5</v>
       </c>
       <c r="J34" s="12">
-        <f>D34*(About!$A$16)/10^6</f>
+        <f>D34*(About!$A$17)/10^6</f>
         <v>9.3156000000000001E-5</v>
       </c>
       <c r="K34" s="12">
-        <f>E34*(About!$A$16)/10^6</f>
+        <f>E34*(About!$A$17)/10^6</f>
         <v>2.0294700000000001E-4</v>
       </c>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="13">
         <v>2041</v>
       </c>
@@ -1991,29 +1918,28 @@
       <c r="E35" s="7">
         <v>186</v>
       </c>
-      <c r="F35" s="13"/>
       <c r="G35" s="1">
         <f t="shared" si="0"/>
         <v>2041</v>
       </c>
       <c r="H35" s="12">
-        <f>B35*(About!$A$16)/10^6</f>
+        <f>B35*(About!$A$17)/10^6</f>
         <v>2.3289E-5</v>
       </c>
       <c r="I35" s="12">
-        <f>C35*(About!$A$16)/10^6</f>
+        <f>C35*(About!$A$17)/10^6</f>
         <v>6.7649000000000002E-5</v>
       </c>
       <c r="J35" s="12">
-        <f>D35*(About!$A$16)/10^6</f>
+        <f>D35*(About!$A$17)/10^6</f>
         <v>9.4265000000000006E-5</v>
       </c>
       <c r="K35" s="12">
-        <f>E35*(About!$A$16)/10^6</f>
+        <f>E35*(About!$A$17)/10^6</f>
         <v>2.06274E-4</v>
       </c>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="13">
         <v>2042</v>
       </c>
@@ -2029,29 +1955,28 @@
       <c r="E36" s="7">
         <v>189</v>
       </c>
-      <c r="F36" s="13"/>
       <c r="G36" s="1">
         <f t="shared" si="0"/>
         <v>2042</v>
       </c>
       <c r="H36" s="12">
-        <f>B36*(About!$A$16)/10^6</f>
+        <f>B36*(About!$A$17)/10^6</f>
         <v>2.4397999999999999E-5</v>
       </c>
       <c r="I36" s="12">
-        <f>C36*(About!$A$16)/10^6</f>
+        <f>C36*(About!$A$17)/10^6</f>
         <v>6.7649000000000002E-5</v>
       </c>
       <c r="J36" s="12">
-        <f>D36*(About!$A$16)/10^6</f>
+        <f>D36*(About!$A$17)/10^6</f>
         <v>9.5373999999999999E-5</v>
       </c>
       <c r="K36" s="12">
-        <f>E36*(About!$A$16)/10^6</f>
+        <f>E36*(About!$A$17)/10^6</f>
         <v>2.0960099999999999E-4</v>
       </c>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="13">
         <v>2043</v>
       </c>
@@ -2067,29 +1992,28 @@
       <c r="E37" s="7">
         <v>192</v>
       </c>
-      <c r="F37" s="13"/>
       <c r="G37" s="1">
         <f t="shared" si="0"/>
         <v>2043</v>
       </c>
       <c r="H37" s="12">
-        <f>B37*(About!$A$16)/10^6</f>
+        <f>B37*(About!$A$17)/10^6</f>
         <v>2.4397999999999999E-5</v>
       </c>
       <c r="I37" s="12">
-        <f>C37*(About!$A$16)/10^6</f>
+        <f>C37*(About!$A$17)/10^6</f>
         <v>6.8757999999999995E-5</v>
       </c>
       <c r="J37" s="12">
-        <f>D37*(About!$A$16)/10^6</f>
+        <f>D37*(About!$A$17)/10^6</f>
         <v>9.6483000000000004E-5</v>
       </c>
       <c r="K37" s="12">
-        <f>E37*(About!$A$16)/10^6</f>
+        <f>E37*(About!$A$17)/10^6</f>
         <v>2.1292800000000001E-4</v>
       </c>
     </row>
-    <row r="38" spans="1:11">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="13">
         <v>2044</v>
       </c>
@@ -2105,29 +2029,28 @@
       <c r="E38" s="7">
         <v>194</v>
       </c>
-      <c r="F38" s="13"/>
       <c r="G38" s="1">
         <f t="shared" si="0"/>
         <v>2044</v>
       </c>
       <c r="H38" s="12">
-        <f>B38*(About!$A$16)/10^6</f>
+        <f>B38*(About!$A$17)/10^6</f>
         <v>2.5506999999999998E-5</v>
       </c>
       <c r="I38" s="12">
-        <f>C38*(About!$A$16)/10^6</f>
+        <f>C38*(About!$A$17)/10^6</f>
         <v>6.9867E-5</v>
       </c>
       <c r="J38" s="12">
-        <f>D38*(About!$A$16)/10^6</f>
+        <f>D38*(About!$A$17)/10^6</f>
         <v>9.7591999999999997E-5</v>
       </c>
       <c r="K38" s="12">
-        <f>E38*(About!$A$16)/10^6</f>
+        <f>E38*(About!$A$17)/10^6</f>
         <v>2.1514599999999999E-4</v>
       </c>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="13">
         <v>2045</v>
       </c>
@@ -2143,29 +2066,28 @@
       <c r="E39" s="7">
         <v>197</v>
       </c>
-      <c r="F39" s="13"/>
       <c r="G39" s="1">
         <f t="shared" si="0"/>
         <v>2045</v>
       </c>
       <c r="H39" s="12">
-        <f>B39*(About!$A$16)/10^6</f>
+        <f>B39*(About!$A$17)/10^6</f>
         <v>2.5506999999999998E-5</v>
       </c>
       <c r="I39" s="12">
-        <f>C39*(About!$A$16)/10^6</f>
+        <f>C39*(About!$A$17)/10^6</f>
         <v>7.0975999999999993E-5</v>
       </c>
       <c r="J39" s="12">
-        <f>D39*(About!$A$16)/10^6</f>
+        <f>D39*(About!$A$17)/10^6</f>
         <v>9.8700999999999989E-5</v>
       </c>
       <c r="K39" s="12">
-        <f>E39*(About!$A$16)/10^6</f>
+        <f>E39*(About!$A$17)/10^6</f>
         <v>2.1847299999999998E-4</v>
       </c>
     </row>
-    <row r="40" spans="1:11">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="13">
         <v>2046</v>
       </c>
@@ -2181,29 +2103,28 @@
       <c r="E40" s="7">
         <v>200</v>
       </c>
-      <c r="F40" s="13"/>
       <c r="G40" s="1">
         <f t="shared" si="0"/>
         <v>2046</v>
       </c>
       <c r="H40" s="12">
-        <f>B40*(About!$A$16)/10^6</f>
+        <f>B40*(About!$A$17)/10^6</f>
         <v>2.6616000000000001E-5</v>
       </c>
       <c r="I40" s="12">
-        <f>C40*(About!$A$16)/10^6</f>
+        <f>C40*(About!$A$17)/10^6</f>
         <v>7.2084999999999998E-5</v>
       </c>
       <c r="J40" s="12">
-        <f>D40*(About!$A$16)/10^6</f>
+        <f>D40*(About!$A$17)/10^6</f>
         <v>9.9810000000000008E-5</v>
       </c>
       <c r="K40" s="12">
-        <f>E40*(About!$A$16)/10^6</f>
+        <f>E40*(About!$A$17)/10^6</f>
         <v>2.2180000000000002E-4</v>
       </c>
     </row>
-    <row r="41" spans="1:11">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="13">
         <v>2047</v>
       </c>
@@ -2219,29 +2140,28 @@
       <c r="E41" s="7">
         <v>203</v>
       </c>
-      <c r="F41" s="13"/>
       <c r="G41" s="1">
         <f t="shared" si="0"/>
         <v>2047</v>
       </c>
       <c r="H41" s="12">
-        <f>B41*(About!$A$16)/10^6</f>
+        <f>B41*(About!$A$17)/10^6</f>
         <v>2.6616000000000001E-5</v>
       </c>
       <c r="I41" s="12">
-        <f>C41*(About!$A$16)/10^6</f>
+        <f>C41*(About!$A$17)/10^6</f>
         <v>7.3194000000000004E-5</v>
       </c>
       <c r="J41" s="12">
-        <f>D41*(About!$A$16)/10^6</f>
+        <f>D41*(About!$A$17)/10^6</f>
         <v>1.0202799999999999E-4</v>
       </c>
       <c r="K41" s="12">
-        <f>E41*(About!$A$16)/10^6</f>
+        <f>E41*(About!$A$17)/10^6</f>
         <v>2.2512700000000001E-4</v>
       </c>
     </row>
-    <row r="42" spans="1:11">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="13">
         <v>2048</v>
       </c>
@@ -2257,29 +2177,28 @@
       <c r="E42" s="7">
         <v>206</v>
       </c>
-      <c r="F42" s="13"/>
       <c r="G42" s="1">
         <f t="shared" si="0"/>
         <v>2048</v>
       </c>
       <c r="H42" s="12">
-        <f>B42*(About!$A$16)/10^6</f>
+        <f>B42*(About!$A$17)/10^6</f>
         <v>2.7725000000000003E-5</v>
       </c>
       <c r="I42" s="12">
-        <f>C42*(About!$A$16)/10^6</f>
+        <f>C42*(About!$A$17)/10^6</f>
         <v>7.4302999999999997E-5</v>
       </c>
       <c r="J42" s="12">
-        <f>D42*(About!$A$16)/10^6</f>
+        <f>D42*(About!$A$17)/10^6</f>
         <v>1.03137E-4</v>
       </c>
       <c r="K42" s="12">
-        <f>E42*(About!$A$16)/10^6</f>
+        <f>E42*(About!$A$17)/10^6</f>
         <v>2.2845400000000001E-4</v>
       </c>
     </row>
-    <row r="43" spans="1:11">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="13">
         <v>2049</v>
       </c>
@@ -2295,29 +2214,28 @@
       <c r="E43" s="7">
         <v>209</v>
       </c>
-      <c r="F43" s="13"/>
       <c r="G43" s="1">
         <f t="shared" si="0"/>
         <v>2049</v>
       </c>
       <c r="H43" s="12">
-        <f>B43*(About!$A$16)/10^6</f>
+        <f>B43*(About!$A$17)/10^6</f>
         <v>2.7725000000000003E-5</v>
       </c>
       <c r="I43" s="12">
-        <f>C43*(About!$A$16)/10^6</f>
+        <f>C43*(About!$A$17)/10^6</f>
         <v>7.5412000000000002E-5</v>
       </c>
       <c r="J43" s="12">
-        <f>D43*(About!$A$16)/10^6</f>
+        <f>D43*(About!$A$17)/10^6</f>
         <v>1.0424599999999999E-4</v>
       </c>
       <c r="K43" s="12">
-        <f>E43*(About!$A$16)/10^6</f>
+        <f>E43*(About!$A$17)/10^6</f>
         <v>2.31781E-4</v>
       </c>
     </row>
-    <row r="44" spans="1:11">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="13">
         <v>2050</v>
       </c>
@@ -2333,25 +2251,24 @@
       <c r="E44" s="7">
         <v>212</v>
       </c>
-      <c r="F44" s="13"/>
       <c r="G44" s="1">
         <f t="shared" si="0"/>
         <v>2050</v>
       </c>
       <c r="H44" s="12">
-        <f>B44*(About!$A$16)/10^6</f>
+        <f>B44*(About!$A$17)/10^6</f>
         <v>2.8833999999999999E-5</v>
       </c>
       <c r="I44" s="12">
-        <f>C44*(About!$A$16)/10^6</f>
+        <f>C44*(About!$A$17)/10^6</f>
         <v>7.6520999999999995E-5</v>
       </c>
       <c r="J44" s="12">
-        <f>D44*(About!$A$16)/10^6</f>
+        <f>D44*(About!$A$17)/10^6</f>
         <v>1.0535500000000001E-4</v>
       </c>
       <c r="K44" s="12">
-        <f>E44*(About!$A$16)/10^6</f>
+        <f>E44*(About!$A$17)/10^6</f>
         <v>2.3510800000000001E-4</v>
       </c>
     </row>
@@ -2361,29 +2278,31 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{842E5F09-E766-5B8D-85AF-A39847EA96FD}"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="13">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
         <f>SourceData!G4</f>
         <v>2010</v>
       </c>
@@ -2392,8 +2311,8 @@
         <v>3.4378999999999997E-5</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="13">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
         <f>SourceData!G5</f>
         <v>2011</v>
       </c>
@@ -2402,8 +2321,8 @@
         <v>3.5487999999999996E-5</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="13">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
         <f>SourceData!G6</f>
         <v>2012</v>
       </c>
@@ -2412,8 +2331,8 @@
         <v>3.6597000000000002E-5</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="13">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
         <f>SourceData!G7</f>
         <v>2013</v>
       </c>
@@ -2422,8 +2341,8 @@
         <v>3.7706000000000001E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="13">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
         <f>SourceData!G8</f>
         <v>2014</v>
       </c>
@@ -2432,8 +2351,8 @@
         <v>3.8815E-5</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="13">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
         <f>SourceData!G9</f>
         <v>2015</v>
       </c>
@@ -2442,8 +2361,8 @@
         <v>3.9923999999999999E-5</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="13">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
         <f>SourceData!G10</f>
         <v>2016</v>
       </c>
@@ -2452,8 +2371,8 @@
         <v>4.2141999999999997E-5</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="13">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
         <f>SourceData!G11</f>
         <v>2017</v>
       </c>
@@ -2462,8 +2381,8 @@
         <v>4.3250999999999996E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="13">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
         <f>SourceData!G12</f>
         <v>2018</v>
       </c>
@@ -2472,8 +2391,8 @@
         <v>4.4360000000000002E-5</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="13">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
         <f>SourceData!G13</f>
         <v>2019</v>
       </c>
@@ -2482,8 +2401,8 @@
         <v>4.5469000000000001E-5</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="13">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
         <f>SourceData!G14</f>
         <v>2020</v>
       </c>
@@ -2492,8 +2411,8 @@
         <v>4.6578E-5</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="13">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
         <f>SourceData!G15</f>
         <v>2021</v>
       </c>
@@ -2502,8 +2421,8 @@
         <v>4.6578E-5</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="13">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
         <f>SourceData!G16</f>
         <v>2022</v>
       </c>
@@ -2512,8 +2431,8 @@
         <v>4.7686999999999999E-5</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="13">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
         <f>SourceData!G17</f>
         <v>2023</v>
       </c>
@@ -2522,8 +2441,8 @@
         <v>4.8795999999999998E-5</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="13">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
         <f>SourceData!G18</f>
         <v>2024</v>
       </c>
@@ -2532,8 +2451,8 @@
         <v>4.9905000000000004E-5</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="13">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
         <f>SourceData!G19</f>
         <v>2025</v>
       </c>
@@ -2542,8 +2461,8 @@
         <v>5.1013999999999996E-5</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="13">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
         <f>SourceData!G20</f>
         <v>2026</v>
       </c>
@@ -2552,8 +2471,8 @@
         <v>5.2122999999999995E-5</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="13">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
         <f>SourceData!G21</f>
         <v>2027</v>
       </c>
@@ -2562,8 +2481,8 @@
         <v>5.3232000000000001E-5</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="13">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
         <f>SourceData!G22</f>
         <v>2028</v>
       </c>
@@ -2572,8 +2491,8 @@
         <v>5.4341E-5</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="13">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
         <f>SourceData!G23</f>
         <v>2029</v>
       </c>
@@ -2582,8 +2501,8 @@
         <v>5.4341E-5</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="13">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
         <f>SourceData!G24</f>
         <v>2030</v>
       </c>
@@ -2592,8 +2511,8 @@
         <v>5.5450000000000006E-5</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="13">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
         <f>SourceData!G25</f>
         <v>2031</v>
       </c>
@@ -2602,8 +2521,8 @@
         <v>5.6558999999999998E-5</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="13">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
         <f>SourceData!G26</f>
         <v>2032</v>
       </c>
@@ -2612,8 +2531,8 @@
         <v>5.7667999999999997E-5</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="13">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
         <f>SourceData!G27</f>
         <v>2033</v>
       </c>
@@ -2622,8 +2541,8 @@
         <v>5.8777000000000003E-5</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="13">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
         <f>SourceData!G28</f>
         <v>2034</v>
       </c>
@@ -2632,8 +2551,8 @@
         <v>5.9885999999999995E-5</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="13">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
         <f>SourceData!G29</f>
         <v>2035</v>
       </c>
@@ -2642,8 +2561,8 @@
         <v>6.0994999999999995E-5</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="13">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
         <f>SourceData!G30</f>
         <v>2036</v>
       </c>
@@ -2652,8 +2571,8 @@
         <v>6.2104E-5</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="13">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
         <f>SourceData!G31</f>
         <v>2037</v>
       </c>
@@ -2662,8 +2581,8 @@
         <v>6.3213000000000006E-5</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="13">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
         <f>SourceData!G32</f>
         <v>2038</v>
       </c>
@@ -2672,8 +2591,8 @@
         <v>6.4321999999999998E-5</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="13">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
         <f>SourceData!G33</f>
         <v>2039</v>
       </c>
@@ -2682,8 +2601,8 @@
         <v>6.5430999999999991E-5</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="13">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
         <f>SourceData!G34</f>
         <v>2040</v>
       </c>
@@ -2692,8 +2611,8 @@
         <v>6.6539999999999997E-5</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="13">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
         <f>SourceData!G35</f>
         <v>2041</v>
       </c>
@@ -2702,8 +2621,8 @@
         <v>6.7649000000000002E-5</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="13">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
         <f>SourceData!G36</f>
         <v>2042</v>
       </c>
@@ -2712,8 +2631,8 @@
         <v>6.7649000000000002E-5</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="13">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
         <f>SourceData!G37</f>
         <v>2043</v>
       </c>
@@ -2722,8 +2641,8 @@
         <v>6.8757999999999995E-5</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="13">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
         <f>SourceData!G38</f>
         <v>2044</v>
       </c>
@@ -2732,8 +2651,8 @@
         <v>6.9867E-5</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="13">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
         <f>SourceData!G39</f>
         <v>2045</v>
       </c>
@@ -2742,8 +2661,8 @@
         <v>7.0975999999999993E-5</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
-      <c r="A38" s="13">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
         <f>SourceData!G40</f>
         <v>2046</v>
       </c>
@@ -2752,8 +2671,8 @@
         <v>7.2084999999999998E-5</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="14.45">
-      <c r="A39" s="13">
+    <row r="39" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A39">
         <f>SourceData!G41</f>
         <v>2047</v>
       </c>
@@ -2762,8 +2681,8 @@
         <v>7.3194000000000004E-5</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="14.45">
-      <c r="A40" s="13">
+    <row r="40" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A40">
         <f>SourceData!G42</f>
         <v>2048</v>
       </c>
@@ -2772,8 +2691,8 @@
         <v>7.4302999999999997E-5</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="14.45">
-      <c r="A41" s="13">
+    <row r="41" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A41">
         <f>SourceData!G43</f>
         <v>2049</v>
       </c>
@@ -2782,8 +2701,8 @@
         <v>7.5412000000000002E-5</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
-      <c r="A42" s="13">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
         <f>SourceData!G44</f>
         <v>2050</v>
       </c>
@@ -2798,24 +2717,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010095990DC6317597479C114DD4E6AB1F33" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="00c0eb7d4c43453177323eb1ac58d7e7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="7889d872-e2a2-4afb-87bc-97561eced75f" xmlns:ns3="c9df191c-55f2-496b-9838-9a5abe4742ad" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b5fe72540fcc493259a136614ad94e00" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -3049,14 +2950,32 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C1C4380-2A0B-4B0D-A718-B224A1BA3880}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0548D816-BA59-436D-B9DE-89256AB3C118}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{418D3AD8-619E-4755-AE2D-49B3D0A24CB3}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E94E7D7-2A7F-4D15-A1E2-9DBDC2ECC08C}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B51FD83F-807D-45C6-B55A-EF33F3603310}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3232902E-9E05-41F9-AFAE-31348E522F2A}"/>
 </file>
</xml_diff>